<commit_message>
11.13. 20:21 기준 업데이트
</commit_message>
<xml_diff>
--- a/모임 장소 설문(응답) 수정.xlsx
+++ b/모임 장소 설문(응답) 수정.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\김지현\filling-good\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samsung\Desktop\강의 등\github\filling good\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F1D9B2-23D2-4F48-BBF9-B46047A70258}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9608009-DE32-48FD-9AD6-220F2F53082D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -382,7 +382,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>PA관 1층 (파관 라운지 / 파관 투썸 앞)</t>
   </si>
@@ -478,6 +478,14 @@
   </si>
   <si>
     <t>장소</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AS관 로비(AS관 5층 공대 휴게실)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>빈 강의실</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -973,15 +981,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA32"/>
+  <dimension ref="A1:AA33"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -1064,7 +1073,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1147,7 +1156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1230,7 +1239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1313,7 +1322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1396,7 +1405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1479,7 +1488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1562,7 +1571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1645,7 +1654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1728,7 +1737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1811,7 +1820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1894,7 +1903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1977,7 +1986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2060,7 +2069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2143,7 +2152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2226,7 +2235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2309,7 +2318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2392,7 +2401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2475,7 +2484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2558,7 +2567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2641,7 +2650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2724,7 +2733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2807,7 +2816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -2890,7 +2899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -2973,7 +2982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -3056,7 +3065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -3139,7 +3148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -3222,7 +3231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -3305,7 +3314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <v>27</v>
       </c>
@@ -3388,7 +3397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -3471,7 +3480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <v>29</v>
       </c>
@@ -3554,7 +3563,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A32" s="2">
         <v>30</v>
       </c>
@@ -3634,6 +3643,89 @@
         <v>0</v>
       </c>
       <c r="AA32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A33" s="2">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>3</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <v>1</v>
+      </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
+      <c r="R33">
+        <v>0</v>
+      </c>
+      <c r="S33">
+        <v>0</v>
+      </c>
+      <c r="T33">
+        <v>0</v>
+      </c>
+      <c r="U33">
+        <v>0</v>
+      </c>
+      <c r="V33">
+        <v>0</v>
+      </c>
+      <c r="W33">
+        <v>0</v>
+      </c>
+      <c r="X33">
+        <v>0</v>
+      </c>
+      <c r="Y33">
+        <v>0</v>
+      </c>
+      <c r="Z33">
+        <v>0</v>
+      </c>
+      <c r="AA33">
         <v>0</v>
       </c>
     </row>
@@ -3649,16 +3741,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8AAD93D-3268-4BB3-B150-E33D629B92FD}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.296875" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="49.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -3684,10 +3778,10 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>13</v>
@@ -3741,7 +3835,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -3749,13 +3843,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="5">
         <v>14</v>
       </c>
       <c r="E2" s="5">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="5">
         <v>11</v>
@@ -3767,7 +3861,7 @@
         <v>6</v>
       </c>
       <c r="I2" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J2" s="5">
         <v>5</v>
@@ -3827,5 +3921,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>